<commit_message>
TCs has been added
</commit_message>
<xml_diff>
--- a/First Part/YallaKora TCs.xlsx
+++ b/First Part/YallaKora TCs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3bsatar\Downloads\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Vodafone Task\First Part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1184D7-6D13-496F-BE35-36479EE989AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4364A8-581E-40BE-BD41-0688F87024CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
   <si>
     <t>TC_ID</t>
   </si>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,6 +920,9 @@
       <c r="F9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Bug Report has been added
</commit_message>
<xml_diff>
--- a/First Part/YallaKora TCs.xlsx
+++ b/First Part/YallaKora TCs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Vodafone Task\First Part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735660E4-36E3-4373-BA35-23AC5FA8E3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF7D7DD-D023-429A-986E-14A65767870D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +351,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -361,7 +369,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,12 +386,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -395,6 +400,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,45 +686,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="55.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="52.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="35.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -723,16 +732,16 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -749,16 +758,16 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -775,16 +784,16 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -801,16 +810,16 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -827,16 +836,16 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -853,16 +862,16 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -879,16 +888,16 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -905,16 +914,16 @@
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -931,16 +940,16 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -957,16 +966,16 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -983,16 +992,16 @@
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1009,16 +1018,16 @@
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1035,16 +1044,16 @@
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1061,16 +1070,16 @@
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1087,16 +1096,16 @@
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1113,16 +1122,16 @@
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F17" s="1" t="s">

</xml_diff>